<commit_message>
PCA explained variance ratio simple visual for appendix
</commit_message>
<xml_diff>
--- a/Data/PCA_results/gua_explained_variance_ratio.xlsx
+++ b/Data/PCA_results/gua_explained_variance_ratio.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hailey/Documents/GitHub/G5055_Practicum_Project2/Data/PCA_results/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{41E933D8-405B-FD45-99CD-5B1676336835}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{88F66A76-5EB4-3048-80AF-B7F85C4C265D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="15820" activeTab="1"/>
   </bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="96">
   <si>
     <t>indicators</t>
   </si>
@@ -2182,12 +2182,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K8" sqref="K8"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="10.83203125" style="4"/>
+    <col min="1" max="1" width="9.1640625" style="4" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="17.5" style="4" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.1640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.1640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.1640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="17.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.2">
@@ -2195,6 +2203,24 @@
         <v>95</v>
       </c>
       <c r="B1" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="H1" s="2" t="s">
         <v>94</v>
       </c>
     </row>
@@ -2764,7 +2790,7 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D1:D1048576">
+  <conditionalFormatting sqref="D2:D1048576">
     <cfRule type="dataBar" priority="1">
       <dataBar>
         <cfvo type="min"/>
@@ -2820,7 +2846,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>D1:D1048576</xm:sqref>
+          <xm:sqref>D2:D1048576</xm:sqref>
         </x14:conditionalFormatting>
       </x14:conditionalFormattings>
     </ext>

</xml_diff>